<commit_message>
Push for log4j update
</commit_message>
<xml_diff>
--- a/ICAAutomation/src/test/resources/ExcelSheets/ICAAutomation_Data.xlsx
+++ b/ICAAutomation/src/test/resources/ExcelSheets/ICAAutomation_Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSTSYS0059\git\ICA\ICAAutomation\src\test\resources\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EF4C6C-46AD-4D28-931A-532465AF35EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45505D66-720B-44D7-955B-737ABDECFC85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="5835" activeTab="1" xr2:uid="{BD6D6DFB-395A-43FF-8F67-EE078B9D8A9E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="5835" xr2:uid="{BD6D6DFB-395A-43FF-8F67-EE078B9D8A9E}"/>
   </bookViews>
   <sheets>
-    <sheet name="EmployerReportForm" sheetId="2" r:id="rId1"/>
-    <sheet name="101_FormValue" sheetId="3" r:id="rId2"/>
+    <sheet name="employerReportFormSubmission" sheetId="2" r:id="rId1"/>
+    <sheet name="formValueValidation" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="102">
   <si>
     <t>TC01</t>
   </si>
@@ -154,15 +154,6 @@
     <t>11/29/2018</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
     <t>Gracy</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>11/25/2018</t>
   </si>
   <si>
@@ -196,9 +184,6 @@
     <t>Head - Eyes</t>
   </si>
   <si>
-    <t>Nothing</t>
-  </si>
-  <si>
     <t>Stone</t>
   </si>
   <si>
@@ -232,28 +217,121 @@
     <t>D:\data.jpg</t>
   </si>
   <si>
+    <t>IMPORTANT NOTE: THIS FORM IS NOT CONSIDERED SUBMITTED AND WILL NOT BE PROCESSED BY THE INDUSTRIAL COMMISSION OF ARIZONA UNTIL SIGNED. TO COMPLETE THE ELECTRONIC SIGNATURE PROCESS, FOLLOW THE INSTRUCTIONS SENT TO THE E-MAIL ADDRESS YOU PROVIDED. THE ELECTRONIC SIGNATURE PROCESS WILL BE AVAILABLE FOR 7 DAYS AFTER A FORM IS SUBMITTED.</t>
+  </si>
+  <si>
+    <t>Thank you for your submission!</t>
+  </si>
+  <si>
+    <t>DisplayTextOne</t>
+  </si>
+  <si>
+    <t>DisplayTextTwo</t>
+  </si>
+  <si>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>Check whether the values are properly submitted in the Employer Report Form</t>
+  </si>
+  <si>
+    <t>$15,963.00</t>
+  </si>
+  <si>
+    <t>12,345</t>
+  </si>
+  <si>
+    <t>Check whether the values are properly mapped from Employer Report form to 101 object in salesforce</t>
+  </si>
+  <si>
+    <t>Street one</t>
+  </si>
+  <si>
+    <t>city one</t>
+  </si>
+  <si>
+    <t>State one</t>
+  </si>
+  <si>
+    <t>Office Street one</t>
+  </si>
+  <si>
+    <t>Office City one</t>
+  </si>
+  <si>
+    <t>Office State one</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>ThankYou</t>
+  </si>
+  <si>
+    <t>ImportantNote</t>
+  </si>
+  <si>
     <t>TC02</t>
   </si>
   <si>
-    <t>IMPORTANT NOTE: THIS FORM IS NOT CONSIDERED SUBMITTED AND WILL NOT BE PROCESSED BY THE INDUSTRIAL COMMISSION OF ARIZONA UNTIL SIGNED. TO COMPLETE THE ELECTRONIC SIGNATURE PROCESS, FOLLOW THE INSTRUCTIONS SENT TO THE E-MAIL ADDRESS YOU PROVIDED. THE ELECTRONIC SIGNATURE PROCESS WILL BE AVAILABLE FOR 7 DAYS AFTER A FORM IS SUBMITTED.</t>
-  </si>
-  <si>
-    <t>Thank you for your submission!</t>
-  </si>
-  <si>
-    <t>DisplayTextOne</t>
-  </si>
-  <si>
-    <t>DisplayTextTwo</t>
-  </si>
-  <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>Check whether the values are properly submitted in the Employer Report Form</t>
-  </si>
-  <si>
-    <t>Check whether the values are properly from Employer Report form to 101 object in salesforce</t>
+    <t>Charan</t>
+  </si>
+  <si>
+    <t>Suzana</t>
+  </si>
+  <si>
+    <t>567-78-7896</t>
+  </si>
+  <si>
+    <t>12/29/2018</t>
+  </si>
+  <si>
+    <t>Street two</t>
+  </si>
+  <si>
+    <t>city two</t>
+  </si>
+  <si>
+    <t>State two</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Chezhiyan</t>
+  </si>
+  <si>
+    <t>56,789</t>
+  </si>
+  <si>
+    <t>Office Street two</t>
+  </si>
+  <si>
+    <t>Office City two</t>
+  </si>
+  <si>
+    <t>Office State two</t>
+  </si>
+  <si>
+    <t>12/25/2018</t>
+  </si>
+  <si>
+    <t>12/26/2018</t>
+  </si>
+  <si>
+    <t>12/27/2018</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Head top</t>
   </si>
 </sst>
 </file>
@@ -296,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,6 +385,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,9 +703,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A495D5-7DCD-4D5C-8FDA-C43C1B8E6C57}">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -639,13 +720,13 @@
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" style="1" customWidth="1"/>
     <col min="19" max="19" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -677,10 +758,10 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -704,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -716,7 +797,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>11</v>
@@ -746,7 +827,7 @@
         <v>19</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>20</v>
@@ -803,10 +884,10 @@
         <v>37</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -814,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -829,13 +910,13 @@
         <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="J2" s="1">
         <v>12345</v>
@@ -844,25 +925,25 @@
         <v>9876543210</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="1">
-        <v>12345</v>
+        <v>44</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="S2" s="1">
         <v>98765</v>
@@ -871,76 +952,210 @@
         <v>9638520741</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="X2" s="1">
         <v>5000</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="1">
+        <v>56789</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1234569870</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="1">
+        <v>12345</v>
+      </c>
+      <c r="T3" s="1">
+        <v>9876589878</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X3" s="1">
+        <v>8000</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AN3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>15963</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>69</v>
+      <c r="AQ3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -951,9 +1166,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B0FFFB-4EBB-44C6-B1C1-2ECEF5570DAE}">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -968,13 +1183,13 @@
     <col min="9" max="9" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="3" customWidth="1"/>
     <col min="19" max="19" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -991,8 +1206,8 @@
     <col min="32" max="32" width="23.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="33.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.85546875" style="3" customWidth="1"/>
+    <col min="36" max="36" width="22.85546875" style="3" customWidth="1"/>
     <col min="37" max="37" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="28.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1006,10 +1221,10 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1033,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -1045,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>11</v>
@@ -1075,7 +1290,7 @@
         <v>19</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>20</v>
@@ -1132,18 +1347,18 @@
         <v>37</v>
       </c>
       <c r="AQ1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="AR1" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -1158,13 +1373,13 @@
         <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="J2" s="1">
         <v>12345</v>
@@ -1173,25 +1388,25 @@
         <v>9876543210</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="1">
-        <v>12345</v>
+        <v>44</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="S2" s="1">
         <v>98765</v>
@@ -1200,76 +1415,210 @@
         <v>9638520741</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="X2" s="1">
         <v>5000</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" s="1" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="1">
+        <v>56789</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1234569870</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="1">
+        <v>12345</v>
+      </c>
+      <c r="T3" s="1">
+        <v>9876589878</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X3" s="1">
+        <v>8000</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AN3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>15963</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>69</v>
+      <c r="AQ3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for parallel execution of test cases
</commit_message>
<xml_diff>
--- a/ICAAutomation/src/test/resources/ExcelSheets/ICAAutomation_Data.xlsx
+++ b/ICAAutomation/src/test/resources/ExcelSheets/ICAAutomation_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSTSYS0059\git\ICA\ICAAutomation\src\test\resources\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45505D66-720B-44D7-955B-737ABDECFC85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83A7877-61BE-42A1-BE61-A9FA15DB4A2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="5835" xr2:uid="{BD6D6DFB-395A-43FF-8F67-EE078B9D8A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="employerReportFormSubmission" sheetId="2" r:id="rId1"/>
     <sheet name="formValueValidation" sheetId="3" r:id="rId2"/>
+    <sheet name="PartOfBodylinkTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
   <si>
     <t>TC01</t>
   </si>
@@ -332,6 +333,78 @@
   </si>
   <si>
     <t>Head top</t>
+  </si>
+  <si>
+    <t>Head - Ear(s)</t>
+  </si>
+  <si>
+    <t>Head - Nose</t>
+  </si>
+  <si>
+    <t>Head - Teeth</t>
+  </si>
+  <si>
+    <t>Head - Mouth</t>
+  </si>
+  <si>
+    <t>Head - Soft Tissue</t>
+  </si>
+  <si>
+    <t>Head - Facial Bones</t>
+  </si>
+  <si>
+    <t>Head - Multiple Neck Injury</t>
+  </si>
+  <si>
+    <t>Head - Vertebrae</t>
+  </si>
+  <si>
+    <t>Head - Multiple Head Injury</t>
+  </si>
+  <si>
+    <t>Head - Skull</t>
+  </si>
+  <si>
+    <t>Head - Brain</t>
+  </si>
+  <si>
+    <t>Check whether the given values are available in Part of Body table</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 3</t>
+  </si>
+  <si>
+    <t>Item 4</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>Item 6</t>
+  </si>
+  <si>
+    <t>Item 7</t>
+  </si>
+  <si>
+    <t>Item 8</t>
+  </si>
+  <si>
+    <t>Item 9</t>
+  </si>
+  <si>
+    <t>Item 10</t>
+  </si>
+  <si>
+    <t>Item 11</t>
+  </si>
+  <si>
+    <t>Item 12</t>
   </si>
 </sst>
 </file>
@@ -374,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -387,6 +460,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -705,7 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A495D5-7DCD-4D5C-8FDA-C43C1B8E6C57}">
   <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1168,7 +1246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B0FFFB-4EBB-44C6-B1C1-2ECEF5570DAE}">
   <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1625,4 +1705,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3B3875-1AAF-4DBF-A7E7-FDEDD38068F2}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="15.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>